<commit_message>
only accounts report filtering left
</commit_message>
<xml_diff>
--- a/public/reports/purchase_order_g.xlsx
+++ b/public/reports/purchase_order_g.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>UNIFORMS &amp; TEXTILE MANUFECTURING CO.</t>
   </si>
@@ -30,19 +30,19 @@
     <t>CUSTOMER:</t>
   </si>
   <si>
-    <t>fayyaz threading co</t>
+    <t>abc</t>
   </si>
   <si>
     <t>LPO REF:</t>
   </si>
   <si>
-    <t>lpo/Affan uniforms co./500</t>
+    <t>lpo/rashid sons/21051</t>
   </si>
   <si>
     <t>ADDRESS:</t>
   </si>
   <si>
-    <t>abc,uae</t>
+    <t>abc,anc</t>
   </si>
   <si>
     <t>Date</t>
@@ -54,13 +54,13 @@
     <t>CONTACT PERSON:</t>
   </si>
   <si>
-    <t>fayyaz</t>
+    <t>SoME VENDOR</t>
   </si>
   <si>
     <t>Payment Date</t>
   </si>
   <si>
-    <t>2019-02-09</t>
+    <t>2019-01-26</t>
   </si>
   <si>
     <t>PHONE</t>
@@ -75,7 +75,7 @@
     <t>PO#</t>
   </si>
   <si>
-    <t>po/fayyaz threading co/2019/4</t>
+    <t>po/abc/2019/6</t>
   </si>
   <si>
     <t>SHIPPING INFO</t>
@@ -87,13 +87,10 @@
     <t>Address</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
-    <t>uae</t>
+    <t>anc</t>
   </si>
   <si>
     <t>Phone</t>
@@ -3870,7 +3867,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -3908,10 +3905,10 @@
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -3949,7 +3946,7 @@
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>15</v>
@@ -3998,22 +3995,22 @@
     </row>
     <row r="17" ht="30" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>27</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="H17" s="22" t="s">
         <v>29</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" ht="20.1" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4031,19 +4028,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25">
-        <v>100.5</v>
+        <v>500</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="26">
-        <v>1507.5</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="20" ht="20.1" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4223,16 +4220,16 @@
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
       <c r="F37" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="29">
-        <v>1507.5</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4244,7 +4241,7 @@
     </row>
     <row r="39" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -4252,7 +4249,7 @@
     </row>
     <row r="40" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H40" s="31"/>
     </row>
@@ -4263,7 +4260,7 @@
     <row r="42" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="F42" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G42" s="35"/>
       <c r="H42" s="31"/>
@@ -4271,7 +4268,7 @@
     <row r="43" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
       <c r="F43" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G43" s="36"/>
       <c r="H43" s="31"/>
@@ -4289,13 +4286,13 @@
     <row r="47" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
       <c r="B47" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H47" s="31"/>
     </row>
     <row r="48" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="37"/>
       <c r="C48" s="37"/>
@@ -4308,7 +4305,7 @@
     </row>
     <row r="49" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -4321,7 +4318,7 @@
     </row>
     <row r="50" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="40"/>
       <c r="C50" s="40"/>

</xml_diff>